<commit_message>
Update Acties workshop 10-02-2020.xlsx
</commit_message>
<xml_diff>
--- a/Workshops/kickoff/Acties workshop 10-02-2020.xlsx
+++ b/Workshops/kickoff/Acties workshop 10-02-2020.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Otto</t>
   </si>
   <si>
-    <t>Info over werdeldwijde definities plus vertaling naar NL</t>
-  </si>
-  <si>
     <t>Input tbv. koppeling tussen de registers</t>
   </si>
   <si>
@@ -131,18 +128,35 @@
     <t>samen emt CBS kennis mbt. internationale categorieen</t>
   </si>
   <si>
-    <t>Gret</t>
-  </si>
-  <si>
     <t>hierarchische doelen-boom</t>
+  </si>
+  <si>
+    <t>Info over wereldwijde definities plus vertaling naar NL</t>
+  </si>
+  <si>
+    <t>Wie</t>
+  </si>
+  <si>
+    <t>Actie</t>
+  </si>
+  <si>
+    <t>Wat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -158,7 +172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -166,13 +180,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -453,271 +484,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="44.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C22" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
-        <v>36</v>
-      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C25">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>